<commit_message>
Signed-off-by: Doug Dmytryk <dougdmytryk@insight-analytical.com>
</commit_message>
<xml_diff>
--- a/AUTOMATION_DATA_SHEET_7 Gens - Karr JJM.xlsx
+++ b/AUTOMATION_DATA_SHEET_7 Gens - Karr JJM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougd\Desktop\git\7Gens_Karr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE3EE71-FE3A-4B80-89F6-A593C7C413A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1339B9-FD7D-45BE-9B34-D670B1C9D2F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58C3B267-3ABF-4EB5-BBD6-7AE44ECDBAEA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="58">
   <si>
     <t>N/A</t>
   </si>
@@ -456,13 +456,52 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -470,63 +509,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -546,26 +528,44 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7551,8 +7551,8 @@
   </sheetPr>
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51:E51"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79:J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7561,60 +7561,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="13"/>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="24"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -7630,27 +7630,27 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="35"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="21"/>
+      <c r="E7" s="24"/>
       <c r="F7" t="s">
         <v>52</v>
       </c>
@@ -7660,20 +7660,20 @@
       <c r="A8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="26"/>
+      <c r="E8" s="31"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="49"/>
+      <c r="E9" s="46"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -7689,44 +7689,44 @@
       <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="55"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="52" t="s">
+      <c r="E11" s="24"/>
+      <c r="F11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="53"/>
-      <c r="H11" s="19" t="s">
+      <c r="G11" s="28"/>
+      <c r="H11" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="21"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="D12" s="50" t="s">
+      <c r="B12" s="20"/>
+      <c r="D12" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="51"/>
-      <c r="F12" s="24" t="s">
+      <c r="E12" s="34"/>
+      <c r="F12" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="22">
+      <c r="G12" s="30"/>
+      <c r="H12" s="35">
         <v>0</v>
       </c>
-      <c r="I12" s="23"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="4" t="s">
         <v>46</v>
       </c>
@@ -7735,17 +7735,17 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="20"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="26">
+      <c r="G13" s="30"/>
+      <c r="H13" s="31">
         <v>10000</v>
       </c>
-      <c r="I13" s="26"/>
+      <c r="I13" s="31"/>
       <c r="J13" s="4" t="s">
         <v>46</v>
       </c>
@@ -7757,102 +7757,102 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="D14" s="19" t="s">
+      <c r="B14" s="20"/>
+      <c r="D14" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="24" t="s">
+      <c r="E14" s="24"/>
+      <c r="F14" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="30">
+      <c r="G14" s="30"/>
+      <c r="H14" s="32">
         <v>-20</v>
       </c>
-      <c r="I14" s="26"/>
+      <c r="I14" s="31"/>
       <c r="J14" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="32"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
       <c r="E15" s="14"/>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="24"/>
-      <c r="H15" s="26">
+      <c r="G15" s="30"/>
+      <c r="H15" s="31">
         <v>110</v>
       </c>
-      <c r="I15" s="26"/>
+      <c r="I15" s="31"/>
       <c r="J15" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="D16" s="19" t="s">
+      <c r="B16" s="20"/>
+      <c r="D16" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="24" t="s">
+      <c r="E16" s="24"/>
+      <c r="F16" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="26" t="s">
+      <c r="G16" s="30"/>
+      <c r="H16" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="I16" s="26"/>
+      <c r="I16" s="31"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="26" t="s">
+      <c r="G17" s="30"/>
+      <c r="H17" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="26"/>
+      <c r="I17" s="31"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="D18" s="19" t="s">
+      <c r="B18" s="20"/>
+      <c r="D18" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="32" t="s">
+      <c r="E18" s="24"/>
+      <c r="F18" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="19" t="s">
+      <c r="G18" s="20"/>
+      <c r="H18" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="21"/>
+      <c r="I18" s="24"/>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -7868,60 +7868,60 @@
       <c r="J20" s="16"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="55"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="52" t="s">
+      <c r="E21" s="24"/>
+      <c r="F21" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="53"/>
-      <c r="H21" s="19" t="s">
+      <c r="G21" s="28"/>
+      <c r="H21" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="21"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="D22" s="50" t="s">
+      <c r="B22" s="20"/>
+      <c r="D22" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="51"/>
-      <c r="F22" s="24" t="s">
+      <c r="E22" s="34"/>
+      <c r="F22" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="22">
+      <c r="G22" s="30"/>
+      <c r="H22" s="35">
         <v>0</v>
       </c>
-      <c r="I22" s="23"/>
+      <c r="I22" s="36"/>
       <c r="J22" s="4"/>
       <c r="K22">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="32"/>
-      <c r="F23" s="24" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="F23" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="25"/>
-      <c r="H23" s="22">
+      <c r="G23" s="52"/>
+      <c r="H23" s="35">
         <v>10000</v>
       </c>
-      <c r="I23" s="23"/>
+      <c r="I23" s="36"/>
       <c r="J23" s="4" t="s">
         <v>46</v>
       </c>
@@ -7933,101 +7933,101 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="D24" s="19" t="s">
+      <c r="B24" s="20"/>
+      <c r="D24" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="24" t="s">
+      <c r="E24" s="24"/>
+      <c r="F24" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="22">
+      <c r="G24" s="30"/>
+      <c r="H24" s="35">
         <v>-20</v>
       </c>
-      <c r="I24" s="23"/>
+      <c r="I24" s="36"/>
       <c r="J24" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
       <c r="E25" s="13"/>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="25"/>
-      <c r="H25" s="22">
+      <c r="G25" s="52"/>
+      <c r="H25" s="35">
         <v>110</v>
       </c>
-      <c r="I25" s="23"/>
+      <c r="I25" s="36"/>
       <c r="J25" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="D26" s="19" t="s">
+      <c r="B26" s="20"/>
+      <c r="D26" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="24" t="s">
+      <c r="E26" s="24"/>
+      <c r="F26" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="26" t="s">
+      <c r="G26" s="30"/>
+      <c r="H26" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="26"/>
+      <c r="I26" s="31"/>
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="32"/>
-      <c r="F27" s="24" t="s">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="F27" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="25"/>
-      <c r="H27" s="26" t="s">
+      <c r="G27" s="52"/>
+      <c r="H27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="26"/>
+      <c r="I27" s="31"/>
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="D28" s="19" t="s">
+      <c r="B28" s="20"/>
+      <c r="D28" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="32" t="s">
+      <c r="E28" s="24"/>
+      <c r="F28" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="32"/>
-      <c r="H28" s="19" t="s">
+      <c r="G28" s="20"/>
+      <c r="H28" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I28" s="21"/>
+      <c r="I28" s="24"/>
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="B29" s="42"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -8043,61 +8043,61 @@
       <c r="J30" s="16"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="55"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="52" t="s">
+      <c r="E31" s="24"/>
+      <c r="F31" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G31" s="53"/>
-      <c r="H31" s="19" t="s">
+      <c r="G31" s="28"/>
+      <c r="H31" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I31" s="20"/>
-      <c r="J31" s="21"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="D32" s="50" t="s">
+      <c r="B32" s="20"/>
+      <c r="D32" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="51"/>
-      <c r="F32" s="24" t="s">
+      <c r="E32" s="34"/>
+      <c r="F32" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="24"/>
-      <c r="H32" s="22">
+      <c r="G32" s="30"/>
+      <c r="H32" s="35">
         <v>0</v>
       </c>
-      <c r="I32" s="23"/>
+      <c r="I32" s="36"/>
       <c r="J32" s="4"/>
       <c r="K32">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="20"/>
       <c r="E33" s="14"/>
-      <c r="F33" s="24" t="s">
+      <c r="F33" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="24"/>
-      <c r="H33" s="26">
+      <c r="G33" s="30"/>
+      <c r="H33" s="31">
         <v>10000</v>
       </c>
-      <c r="I33" s="26"/>
+      <c r="I33" s="31"/>
       <c r="J33" s="4" t="s">
         <v>46</v>
       </c>
@@ -8109,100 +8109,100 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="32"/>
-      <c r="D34" s="19" t="s">
+      <c r="B34" s="20"/>
+      <c r="D34" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="21"/>
-      <c r="F34" s="24" t="s">
+      <c r="E34" s="24"/>
+      <c r="F34" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="24"/>
-      <c r="H34" s="30">
+      <c r="G34" s="30"/>
+      <c r="H34" s="32">
         <v>-20</v>
       </c>
-      <c r="I34" s="26"/>
+      <c r="I34" s="31"/>
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" s="32"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
       <c r="E35" s="14"/>
-      <c r="F35" s="24" t="s">
+      <c r="F35" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G35" s="24"/>
-      <c r="H35" s="26">
+      <c r="G35" s="30"/>
+      <c r="H35" s="31">
         <v>110</v>
       </c>
-      <c r="I35" s="26"/>
+      <c r="I35" s="31"/>
       <c r="J35" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="D36" s="19" t="s">
+      <c r="B36" s="20"/>
+      <c r="D36" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="24" t="s">
+      <c r="E36" s="24"/>
+      <c r="F36" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G36" s="24"/>
-      <c r="H36" s="26" t="s">
+      <c r="G36" s="30"/>
+      <c r="H36" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="I36" s="26"/>
+      <c r="I36" s="31"/>
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="32"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="E37" s="14"/>
-      <c r="F37" s="24" t="s">
+      <c r="F37" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="24"/>
-      <c r="H37" s="26" t="s">
+      <c r="G37" s="30"/>
+      <c r="H37" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="I37" s="26"/>
+      <c r="I37" s="31"/>
       <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="D38" s="19" t="s">
+      <c r="B38" s="20"/>
+      <c r="D38" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E38" s="21"/>
-      <c r="F38" s="32" t="s">
+      <c r="E38" s="24"/>
+      <c r="F38" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G38" s="32"/>
-      <c r="H38" s="19" t="s">
+      <c r="G38" s="20"/>
+      <c r="H38" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I38" s="21"/>
+      <c r="I38" s="24"/>
       <c r="J38" s="4"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
-      <c r="B39" s="42"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="14"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
       <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -8218,55 +8218,55 @@
       <c r="J40" s="16"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="54" t="s">
+      <c r="A41" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="55"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="52" t="s">
+      <c r="D41" s="23"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G41" s="53"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="21"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="24"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="32"/>
-      <c r="D42" s="19" t="s">
+      <c r="B42" s="20"/>
+      <c r="D42" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="24" t="s">
+      <c r="E42" s="24"/>
+      <c r="F42" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="24"/>
-      <c r="H42" s="30">
+      <c r="G42" s="30"/>
+      <c r="H42" s="32">
         <v>0</v>
       </c>
-      <c r="I42" s="26"/>
+      <c r="I42" s="31"/>
       <c r="J42" s="4"/>
       <c r="K42">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="32"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="20"/>
       <c r="E43" s="14"/>
-      <c r="F43" s="24" t="s">
+      <c r="F43" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G43" s="24"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
       <c r="J43" s="4" t="s">
         <v>46</v>
       </c>
@@ -8278,122 +8278,122 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="32"/>
-      <c r="D44" s="19" t="s">
+      <c r="B44" s="20"/>
+      <c r="D44" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E44" s="21"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G44" s="24"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="26"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="31"/>
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
-      <c r="B45" s="32"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="20"/>
       <c r="E45" s="14"/>
-      <c r="F45" s="24" t="s">
+      <c r="F45" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G45" s="24"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
       <c r="J45" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="32"/>
-      <c r="D46" s="19" t="s">
+      <c r="B46" s="20"/>
+      <c r="D46" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="21"/>
-      <c r="F46" s="24" t="s">
+      <c r="E46" s="24"/>
+      <c r="F46" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G46" s="24"/>
-      <c r="H46" s="26" t="s">
+      <c r="G46" s="30"/>
+      <c r="H46" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="I46" s="26"/>
+      <c r="I46" s="31"/>
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
-      <c r="B47" s="32"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="20"/>
       <c r="E47" s="14"/>
-      <c r="F47" s="24" t="s">
+      <c r="F47" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G47" s="24"/>
-      <c r="H47" s="26" t="s">
+      <c r="G47" s="30"/>
+      <c r="H47" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="I47" s="26"/>
+      <c r="I47" s="31"/>
       <c r="J47" s="4"/>
     </row>
     <row r="48" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="32"/>
-      <c r="D48" s="19" t="s">
+      <c r="B48" s="20"/>
+      <c r="D48" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E48" s="21"/>
-      <c r="F48" s="32" t="s">
+      <c r="E48" s="24"/>
+      <c r="F48" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G48" s="32"/>
-      <c r="H48" s="19" t="s">
+      <c r="G48" s="20"/>
+      <c r="H48" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="I48" s="21"/>
+      <c r="I48" s="24"/>
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="41"/>
-      <c r="B49" s="42"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="22"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="14"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="s">
+      <c r="A50" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="29"/>
+      <c r="B50" s="54"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="55"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="23" t="s">
+      <c r="D51" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E51" s="23"/>
+      <c r="E51" s="36"/>
       <c r="J51" s="4"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -8410,13 +8410,13 @@
       <c r="E53" t="s">
         <v>28</v>
       </c>
-      <c r="F53" s="19" t="s">
+      <c r="F53" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="21"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="24"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
@@ -8431,27 +8431,27 @@
       <c r="E55" t="s">
         <v>28</v>
       </c>
-      <c r="F55" s="26" t="s">
+      <c r="F55" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="26"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="31"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="27" t="s">
+      <c r="A56" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="28"/>
-      <c r="H56" s="28"/>
-      <c r="I56" s="28"/>
-      <c r="J56" s="29"/>
+      <c r="B56" s="54"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="54"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="54"/>
+      <c r="H56" s="54"/>
+      <c r="I56" s="54"/>
+      <c r="J56" s="55"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
@@ -8461,43 +8461,43 @@
       <c r="C57" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D57" s="38" t="str">
+      <c r="D57" s="49" t="str">
         <f>D11</f>
         <v>40AIT-400</v>
       </c>
-      <c r="E57" s="39"/>
+      <c r="E57" s="50"/>
       <c r="G57" s="12" t="s">
         <v>25</v>
       </c>
       <c r="H57" t="s">
         <v>22</v>
       </c>
-      <c r="I57" s="36" t="str">
+      <c r="I57" s="47" t="str">
         <f>D21</f>
         <v>50-AIT-400</v>
       </c>
-      <c r="J57" s="40"/>
+      <c r="J57" s="51"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C58" s="19" t="str">
+      <c r="C58" s="23" t="str">
         <f>H11</f>
         <v>Condy</v>
       </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="21"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="24"/>
       <c r="G58" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H58" s="19" t="str">
+      <c r="H58" s="23" t="str">
         <f>H21</f>
         <v>Condy</v>
       </c>
-      <c r="I58" s="20"/>
-      <c r="J58" s="21"/>
+      <c r="I58" s="29"/>
+      <c r="J58" s="24"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
@@ -8661,11 +8661,11 @@
       <c r="C78" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D78" s="36" t="str">
+      <c r="D78" s="47" t="str">
         <f>D31</f>
         <v>60-AIT-400</v>
       </c>
-      <c r="E78" s="37"/>
+      <c r="E78" s="48"/>
       <c r="F78" s="11"/>
       <c r="G78" s="10" t="s">
         <v>23</v>
@@ -8673,30 +8673,32 @@
       <c r="H78" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I78" s="38"/>
-      <c r="J78" s="39"/>
+      <c r="I78" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="J78" s="50"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C79" s="19" t="str">
+      <c r="C79" s="23" t="str">
         <f>H31</f>
         <v>Condy</v>
       </c>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
       <c r="F79" s="5"/>
       <c r="G79" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H79" s="19">
+      <c r="H79" s="23">
         <f>H41</f>
         <v>0</v>
       </c>
-      <c r="I79" s="20"/>
-      <c r="J79" s="21"/>
+      <c r="I79" s="29"/>
+      <c r="J79" s="24"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
@@ -8871,18 +8873,18 @@
       <c r="J98" s="1"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="33" t="s">
+      <c r="A102" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B102" s="34"/>
-      <c r="C102" s="34"/>
-      <c r="D102" s="34"/>
-      <c r="E102" s="34"/>
-      <c r="F102" s="34"/>
-      <c r="G102" s="34"/>
-      <c r="H102" s="34"/>
-      <c r="I102" s="34"/>
-      <c r="J102" s="35"/>
+      <c r="B102" s="44"/>
+      <c r="C102" s="44"/>
+      <c r="D102" s="44"/>
+      <c r="E102" s="44"/>
+      <c r="F102" s="44"/>
+      <c r="G102" s="44"/>
+      <c r="H102" s="44"/>
+      <c r="I102" s="44"/>
+      <c r="J102" s="45"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
@@ -9025,6 +9027,107 @@
     </row>
   </sheetData>
   <mergeCells count="125">
+    <mergeCell ref="H58:J58"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F53:J53"/>
+    <mergeCell ref="F55:J55"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A50:J50"/>
+    <mergeCell ref="A56:J56"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="A36:B37"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="A102:J102"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="H79:J79"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A28:B29"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G29"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="A26:B27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="A34:B35"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="A38:B39"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G39"/>
+    <mergeCell ref="H38:I38"/>
     <mergeCell ref="A48:B49"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="F48:G49"/>
@@ -9049,107 +9152,6 @@
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
     <mergeCell ref="H42:I42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="A38:B39"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G39"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="F18:G19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A102:J102"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="I78:J78"/>
-    <mergeCell ref="H79:J79"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G29"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="A26:B27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="H58:J58"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F53:J53"/>
-    <mergeCell ref="F55:J55"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A50:J50"/>
-    <mergeCell ref="A56:J56"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="A36:B37"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="A32:B33"/>
   </mergeCells>
   <dataValidations count="11">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D48:E48 D18:E18 D38:E38" xr:uid="{BA6AE503-FE5D-4A1A-B5FF-C58DE9EF8707}">

</xml_diff>